<commit_message>
Redo supervision, incl. distinctions
</commit_message>
<xml_diff>
--- a/data/supervision_en.xlsx
+++ b/data/supervision_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA88F55-6898-4715-AF23-1028D041DC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B621CBD-7074-452C-97C3-6800524B4933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3150" yWindow="4350" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supervision" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>what</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Music Pedagogy</t>
   </si>
   <si>
-    <t>PhD in Neuroscience</t>
-  </si>
-  <si>
     <t>2013 - 2014</t>
   </si>
   <si>
@@ -67,12 +64,6 @@
     <t>Professional Doctorate in Counselling Psychology</t>
   </si>
   <si>
-    <t>Psychological Research Methods (Evolutionary Psychology) MSc</t>
-  </si>
-  <si>
-    <t>MSc in Psychology</t>
-  </si>
-  <si>
     <t>Since 2015</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>Andrés Felipe Orozco Serrato (2020 - 2021)</t>
   </si>
   <si>
-    <t>Andrés Castellanos-Chacón (2017 - 2018; teaching supervision 2019 - Present)</t>
-  </si>
-  <si>
     <t>Paula Andrea Betancourt Velandia  (2018 - 2019)</t>
   </si>
   <si>
@@ -127,27 +115,9 @@
     <t>Haydn Ricardo Roldán Morales (2015 - 2016)</t>
   </si>
   <si>
-    <t>Maria Alejandra Abello Mozo  (2017 - 2018)</t>
-  </si>
-  <si>
-    <t>Natalia Elízabeth Moreno Buitrago (2017 ‑ 2019)</t>
-  </si>
-  <si>
-    <t>Juan Felipe Pérez Ariza (2017 ‑ 2019)</t>
-  </si>
-  <si>
     <t>John Jairo Rubio (2021 - 2022)</t>
   </si>
   <si>
-    <t>Mariana Saavedra Botero (2021 - 2022)</t>
-  </si>
-  <si>
-    <t>Daniela Martínez Franco (2021 - 2022)</t>
-  </si>
-  <si>
-    <t>Angie Alejandra Lozano Sanjuan (2021 - 2022)</t>
-  </si>
-  <si>
     <t>\href{https://www.uel.ac.uk/}{University of East London}, UK</t>
   </si>
   <si>
@@ -160,19 +130,55 @@
     <t>\href{https://www.upn.edu.co/}{Universidad Pedagógica Nacional}, Colombia</t>
   </si>
   <si>
+    <t>\href{https://www.researchgate.net/profile/Francisco-Flores-14}{Francisco Javier Flores}. Supervised together with Lisa Chiara Fellin</t>
+  </si>
+  <si>
+    <t>\href{https://www.uv.es/}{Universitat de València}, Spain</t>
+  </si>
+  <si>
+    <t>Maria Alejandra Abello Mozo  (2017 - 2018)  - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Natalia Elízabeth Moreno Buitrago (2017 ‑ 2019)  - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Juan Felipe Pérez Ariza (2017 ‑ 2019)  - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Angie Alejandra Lozano Sanjuan (2021 - 2022) - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Daniela Martínez Franco (2021 - 2022) - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Mariana Saavedra Botero (2021 - 2022) - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Maria Daniela Martínez Luna (2020 - 2021)  - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Juan Sebastián Preciado Ruíz (2020 - 2021)  - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>Andrés Castellanos-Chacón (2017 -2018) - \textbf{\textit{Distinction}}. Teaching supervision (2019 - Present)</t>
+  </si>
+  <si>
     <t>\href{https://www.researchgate.net/profile/Milena-Vasquez-Amezquita}{Milena Vásquez-Amézquita}. Supervised together with  Alicia Salvador</t>
   </si>
   <si>
+    <t>PhD in Neuroscience  - \textbf{\textit{Summa Cum Laude}}</t>
+  </si>
+  <si>
+    <t>Julia Sanz-Vidania. Supervised together with \href{https://www.scraigroberts.com/}{S Craig Roberts}</t>
+  </si>
+  <si>
+    <t>Psychological Research Methods (Evolutionary Psychology) MSc - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
+    <t>MSc in Psychology - \textbf{\textit{Distinction}}</t>
+  </si>
+  <si>
     <t>Adrián Acosta Guerrero. Supervised together with \href{https://www.researchgate.net/profile/Milena-Vasquez-Amezquita}{Milena Vásquez-Amézquita}</t>
-  </si>
-  <si>
-    <t>\href{https://www.researchgate.net/profile/Francisco-Flores-14}{Francisco Javier Flores}. Supervised together with Lisa Chiara Fellin</t>
-  </si>
-  <si>
-    <t>Julia Sanz-Vidania. Supervised together with \href{https://www.scraigroberts.com/}{S Craig Roberts}</t>
-  </si>
-  <si>
-    <t>\href{https://www.uv.es/}{Universitat de València}, Spain</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,46 +1062,46 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>49</v>
@@ -1103,17 +1109,17 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1121,14 +1127,14 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1136,14 +1142,14 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1151,7 +1157,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1159,16 +1165,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,7 +1190,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,7 +1198,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1200,7 +1206,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1214,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,7 +1222,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1224,7 +1230,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1232,7 +1238,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -1240,17 +1246,15 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1258,15 +1262,17 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -1274,7 +1280,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1282,7 +1288,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1290,7 +1296,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -1298,7 +1304,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1306,20 +1312,24 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
@@ -1380,6 +1390,18 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>